<commit_message>
V1.4 Correction ortographique + modification fonction Est_Mort() + verrouillage menu triche
</commit_message>
<xml_diff>
--- a/docs/Projet_RED.xlsx
+++ b/docs/Projet_RED.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/425d26859fa2f4c4/Documents/Cours (2022-2023)/Projet/projet_red/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2655EF56831DC8942C3404C0444974D38B18554A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F1CD2E-C58F-41AD-8C70-858C20B01DA9}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2655EF56831DC8942C3404C0444974D38B18554A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4015969-BF69-4D25-95BD-9926D7D52ACA}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
@@ -192,6 +192,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="1"/>
     </font>
@@ -248,10 +255,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -265,7 +273,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -280,8 +288,12 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,7 +609,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -692,7 +704,7 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="5">
@@ -1025,6 +1037,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{AFBB8EF7-0F19-435B-846C-2EFE9A4AC09F}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>